<commit_message>
WAC ok + filtres sur la distance + bugfix nan
</commit_message>
<xml_diff>
--- a/Xports/UD_French-FQB/VERB-indirect-obj.xlsx
+++ b/Xports/UD_French-FQB/VERB-indirect-obj.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="72">
   <si>
     <t>sent_id</t>
   </si>
@@ -56,6 +56,9 @@
   </si>
   <si>
     <t>MISC</t>
+  </si>
+  <si>
+    <t>dist</t>
   </si>
   <si>
     <t>FQB_CLEF03-118</t>
@@ -584,13 +587,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N10"/>
+  <dimension ref="A1:O10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -633,395 +636,425 @@
       <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:15">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" t="s">
+        <v>53</v>
+      </c>
+      <c r="H2" t="s">
+        <v>59</v>
+      </c>
+      <c r="I2" t="s">
+        <v>60</v>
+      </c>
+      <c r="J2" t="s">
+        <v>61</v>
+      </c>
+      <c r="K2" t="s">
+        <v>49</v>
+      </c>
+      <c r="L2" t="s">
+        <v>67</v>
+      </c>
+      <c r="M2" t="s">
+        <v>60</v>
+      </c>
+      <c r="N2" t="s">
+        <v>60</v>
+      </c>
+      <c r="O2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" t="s">
+        <v>54</v>
+      </c>
+      <c r="H3" t="s">
+        <v>59</v>
+      </c>
+      <c r="I3" t="s">
+        <v>60</v>
+      </c>
+      <c r="J3" t="s">
+        <v>61</v>
+      </c>
+      <c r="K3" t="s">
+        <v>51</v>
+      </c>
+      <c r="L3" t="s">
+        <v>67</v>
+      </c>
+      <c r="M3" t="s">
+        <v>60</v>
+      </c>
+      <c r="N3" t="s">
+        <v>60</v>
+      </c>
+      <c r="O3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I4" t="s">
+        <v>60</v>
+      </c>
+      <c r="J4" t="s">
+        <v>62</v>
+      </c>
+      <c r="K4" t="s">
+        <v>51</v>
+      </c>
+      <c r="L4" t="s">
+        <v>68</v>
+      </c>
+      <c r="M4" t="s">
+        <v>60</v>
+      </c>
+      <c r="N4" t="s">
+        <v>60</v>
+      </c>
+      <c r="O4">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" t="s">
+        <v>55</v>
+      </c>
+      <c r="H5" t="s">
+        <v>59</v>
+      </c>
+      <c r="I5" t="s">
+        <v>60</v>
+      </c>
+      <c r="J5" t="s">
+        <v>63</v>
+      </c>
+      <c r="K5" t="s">
+        <v>52</v>
+      </c>
+      <c r="L5" t="s">
+        <v>69</v>
+      </c>
+      <c r="M5" t="s">
+        <v>60</v>
+      </c>
+      <c r="N5" t="s">
+        <v>60</v>
+      </c>
+      <c r="O5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E6" t="s">
+        <v>49</v>
+      </c>
+      <c r="F6" t="s">
+        <v>35</v>
+      </c>
+      <c r="G6" t="s">
+        <v>56</v>
+      </c>
+      <c r="H6" t="s">
+        <v>59</v>
+      </c>
+      <c r="I6" t="s">
+        <v>60</v>
+      </c>
+      <c r="J6" t="s">
+        <v>61</v>
+      </c>
+      <c r="K6" t="s">
+        <v>66</v>
+      </c>
+      <c r="L6" t="s">
+        <v>70</v>
+      </c>
+      <c r="M6" t="s">
+        <v>60</v>
+      </c>
+      <c r="N6" t="s">
+        <v>60</v>
+      </c>
+      <c r="O6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F7" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" t="s">
+        <v>57</v>
+      </c>
+      <c r="H7" t="s">
+        <v>59</v>
+      </c>
+      <c r="I7" t="s">
+        <v>60</v>
+      </c>
+      <c r="J7" t="s">
+        <v>64</v>
+      </c>
+      <c r="K7" t="s">
+        <v>66</v>
+      </c>
+      <c r="L7" t="s">
+        <v>70</v>
+      </c>
+      <c r="M7" t="s">
+        <v>60</v>
+      </c>
+      <c r="N7" t="s">
+        <v>71</v>
+      </c>
+      <c r="O7">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" t="s">
+        <v>45</v>
+      </c>
+      <c r="E8" t="s">
+        <v>51</v>
+      </c>
+      <c r="F8" t="s">
+        <v>37</v>
+      </c>
+      <c r="G8" t="s">
+        <v>37</v>
+      </c>
+      <c r="H8" t="s">
+        <v>59</v>
+      </c>
+      <c r="I8" t="s">
+        <v>60</v>
+      </c>
+      <c r="J8" t="s">
+        <v>62</v>
+      </c>
+      <c r="K8" t="s">
+        <v>50</v>
+      </c>
+      <c r="L8" t="s">
+        <v>68</v>
+      </c>
+      <c r="M8" t="s">
+        <v>60</v>
+      </c>
+      <c r="N8" t="s">
+        <v>60</v>
+      </c>
+      <c r="O8">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E9" t="s">
+        <v>52</v>
+      </c>
+      <c r="F9" t="s">
+        <v>38</v>
+      </c>
+      <c r="G9" t="s">
+        <v>58</v>
+      </c>
+      <c r="H9" t="s">
+        <v>59</v>
+      </c>
+      <c r="I9" t="s">
+        <v>60</v>
+      </c>
+      <c r="J9" t="s">
+        <v>65</v>
+      </c>
+      <c r="K9" t="s">
+        <v>66</v>
+      </c>
+      <c r="L9" t="s">
+        <v>70</v>
+      </c>
+      <c r="M9" t="s">
+        <v>60</v>
+      </c>
+      <c r="N9" t="s">
+        <v>60</v>
+      </c>
+      <c r="O9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="A10" t="s">
         <v>23</v>
       </c>
-      <c r="C2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="C10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" t="s">
         <v>47</v>
       </c>
-      <c r="F2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G2" t="s">
-        <v>52</v>
-      </c>
-      <c r="H2" t="s">
-        <v>58</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="E10" t="s">
+        <v>50</v>
+      </c>
+      <c r="F10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G10" t="s">
+        <v>57</v>
+      </c>
+      <c r="H10" t="s">
         <v>59</v>
       </c>
-      <c r="J2" t="s">
-        <v>60</v>
-      </c>
-      <c r="K2" t="s">
-        <v>48</v>
-      </c>
-      <c r="L2" t="s">
+      <c r="I10" t="s">
+        <v>60</v>
+      </c>
+      <c r="J10" t="s">
+        <v>64</v>
+      </c>
+      <c r="K10" t="s">
         <v>66</v>
       </c>
-      <c r="M2" t="s">
-        <v>59</v>
-      </c>
-      <c r="N2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E3" t="s">
-        <v>48</v>
-      </c>
-      <c r="F3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G3" t="s">
-        <v>53</v>
-      </c>
-      <c r="H3" t="s">
-        <v>58</v>
-      </c>
-      <c r="I3" t="s">
-        <v>59</v>
-      </c>
-      <c r="J3" t="s">
-        <v>60</v>
-      </c>
-      <c r="K3" t="s">
-        <v>50</v>
-      </c>
-      <c r="L3" t="s">
-        <v>66</v>
-      </c>
-      <c r="M3" t="s">
-        <v>59</v>
-      </c>
-      <c r="N3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14">
-      <c r="A4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D4" t="s">
-        <v>40</v>
-      </c>
-      <c r="E4" t="s">
-        <v>48</v>
-      </c>
-      <c r="F4" t="s">
-        <v>32</v>
-      </c>
-      <c r="G4" t="s">
-        <v>32</v>
-      </c>
-      <c r="H4" t="s">
-        <v>58</v>
-      </c>
-      <c r="I4" t="s">
-        <v>59</v>
-      </c>
-      <c r="J4" t="s">
-        <v>61</v>
-      </c>
-      <c r="K4" t="s">
-        <v>50</v>
-      </c>
-      <c r="L4" t="s">
-        <v>67</v>
-      </c>
-      <c r="M4" t="s">
-        <v>59</v>
-      </c>
-      <c r="N4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14">
-      <c r="A5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D5" t="s">
-        <v>41</v>
-      </c>
-      <c r="E5" t="s">
-        <v>48</v>
-      </c>
-      <c r="F5" t="s">
-        <v>33</v>
-      </c>
-      <c r="G5" t="s">
-        <v>54</v>
-      </c>
-      <c r="H5" t="s">
-        <v>58</v>
-      </c>
-      <c r="I5" t="s">
-        <v>59</v>
-      </c>
-      <c r="J5" t="s">
-        <v>62</v>
-      </c>
-      <c r="K5" t="s">
-        <v>51</v>
-      </c>
-      <c r="L5" t="s">
-        <v>68</v>
-      </c>
-      <c r="M5" t="s">
-        <v>59</v>
-      </c>
-      <c r="N5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14">
-      <c r="A6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D6" t="s">
-        <v>42</v>
-      </c>
-      <c r="E6" t="s">
-        <v>48</v>
-      </c>
-      <c r="F6" t="s">
-        <v>34</v>
-      </c>
-      <c r="G6" t="s">
-        <v>55</v>
-      </c>
-      <c r="H6" t="s">
-        <v>58</v>
-      </c>
-      <c r="I6" t="s">
-        <v>59</v>
-      </c>
-      <c r="J6" t="s">
-        <v>60</v>
-      </c>
-      <c r="K6" t="s">
-        <v>65</v>
-      </c>
-      <c r="L6" t="s">
-        <v>69</v>
-      </c>
-      <c r="M6" t="s">
-        <v>59</v>
-      </c>
-      <c r="N6" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14">
-      <c r="A7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D7" t="s">
-        <v>43</v>
-      </c>
-      <c r="E7" t="s">
-        <v>49</v>
-      </c>
-      <c r="F7" t="s">
-        <v>35</v>
-      </c>
-      <c r="G7" t="s">
-        <v>56</v>
-      </c>
-      <c r="H7" t="s">
-        <v>58</v>
-      </c>
-      <c r="I7" t="s">
-        <v>59</v>
-      </c>
-      <c r="J7" t="s">
-        <v>63</v>
-      </c>
-      <c r="K7" t="s">
-        <v>65</v>
-      </c>
-      <c r="L7" t="s">
-        <v>69</v>
-      </c>
-      <c r="M7" t="s">
-        <v>59</v>
-      </c>
-      <c r="N7" t="s">
+      <c r="L10" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="8" spans="1:14">
-      <c r="A8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" t="s">
-        <v>36</v>
-      </c>
-      <c r="D8" t="s">
-        <v>44</v>
-      </c>
-      <c r="E8" t="s">
-        <v>50</v>
-      </c>
-      <c r="F8" t="s">
-        <v>36</v>
-      </c>
-      <c r="G8" t="s">
-        <v>36</v>
-      </c>
-      <c r="H8" t="s">
-        <v>58</v>
-      </c>
-      <c r="I8" t="s">
-        <v>59</v>
-      </c>
-      <c r="J8" t="s">
-        <v>61</v>
-      </c>
-      <c r="K8" t="s">
-        <v>49</v>
-      </c>
-      <c r="L8" t="s">
-        <v>67</v>
-      </c>
-      <c r="M8" t="s">
-        <v>59</v>
-      </c>
-      <c r="N8" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14">
-      <c r="A9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" t="s">
-        <v>37</v>
-      </c>
-      <c r="D9" t="s">
-        <v>45</v>
-      </c>
-      <c r="E9" t="s">
-        <v>51</v>
-      </c>
-      <c r="F9" t="s">
-        <v>37</v>
-      </c>
-      <c r="G9" t="s">
-        <v>57</v>
-      </c>
-      <c r="H9" t="s">
-        <v>58</v>
-      </c>
-      <c r="I9" t="s">
-        <v>59</v>
-      </c>
-      <c r="J9" t="s">
-        <v>64</v>
-      </c>
-      <c r="K9" t="s">
-        <v>65</v>
-      </c>
-      <c r="L9" t="s">
-        <v>69</v>
-      </c>
-      <c r="M9" t="s">
-        <v>59</v>
-      </c>
-      <c r="N9" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14">
-      <c r="A10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" t="s">
-        <v>35</v>
-      </c>
-      <c r="D10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E10" t="s">
-        <v>49</v>
-      </c>
-      <c r="F10" t="s">
-        <v>35</v>
-      </c>
-      <c r="G10" t="s">
-        <v>56</v>
-      </c>
-      <c r="H10" t="s">
-        <v>58</v>
-      </c>
-      <c r="I10" t="s">
-        <v>59</v>
-      </c>
-      <c r="J10" t="s">
-        <v>63</v>
-      </c>
-      <c r="K10" t="s">
-        <v>65</v>
-      </c>
-      <c r="L10" t="s">
-        <v>69</v>
-      </c>
       <c r="M10" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="N10" t="s">
-        <v>70</v>
+        <v>71</v>
+      </c>
+      <c r="O10">
+        <v>-1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
WIP on ConnluSent & ConnluLine
</commit_message>
<xml_diff>
--- a/Xports/UD_French-FQB/VERB-indirect-obj.xlsx
+++ b/Xports/UD_French-FQB/VERB-indirect-obj.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="71">
   <si>
     <t>sent_id</t>
   </si>
@@ -56,9 +56,6 @@
   </si>
   <si>
     <t>MISC</t>
-  </si>
-  <si>
-    <t>dist</t>
   </si>
   <si>
     <t>FQB_CLEF03-118</t>
@@ -587,13 +584,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O10"/>
+  <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -636,425 +633,395 @@
       <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" t="s">
         <v>14</v>
       </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G2" t="s">
+        <v>52</v>
+      </c>
+      <c r="H2" t="s">
+        <v>58</v>
+      </c>
+      <c r="I2" t="s">
+        <v>59</v>
+      </c>
+      <c r="J2" t="s">
+        <v>60</v>
+      </c>
+      <c r="K2" t="s">
+        <v>48</v>
+      </c>
+      <c r="L2" t="s">
+        <v>66</v>
+      </c>
+      <c r="M2" t="s">
+        <v>59</v>
+      </c>
+      <c r="N2" t="s">
+        <v>59</v>
+      </c>
     </row>
-    <row r="2" spans="1:15">
-      <c r="A2" t="s">
+    <row r="3" spans="1:14">
+      <c r="A3" t="s">
         <v>15</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>24</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C3" t="s">
         <v>31</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D3" t="s">
         <v>39</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E3" t="s">
         <v>48</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F3" t="s">
         <v>31</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G3" t="s">
         <v>53</v>
       </c>
-      <c r="H2" t="s">
-        <v>59</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="H3" t="s">
+        <v>58</v>
+      </c>
+      <c r="I3" t="s">
+        <v>59</v>
+      </c>
+      <c r="J3" t="s">
         <v>60</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K3" t="s">
+        <v>50</v>
+      </c>
+      <c r="L3" t="s">
+        <v>66</v>
+      </c>
+      <c r="M3" t="s">
+        <v>59</v>
+      </c>
+      <c r="N3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H4" t="s">
+        <v>58</v>
+      </c>
+      <c r="I4" t="s">
+        <v>59</v>
+      </c>
+      <c r="J4" t="s">
         <v>61</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K4" t="s">
+        <v>50</v>
+      </c>
+      <c r="L4" t="s">
+        <v>67</v>
+      </c>
+      <c r="M4" t="s">
+        <v>59</v>
+      </c>
+      <c r="N4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G5" t="s">
+        <v>54</v>
+      </c>
+      <c r="H5" t="s">
+        <v>58</v>
+      </c>
+      <c r="I5" t="s">
+        <v>59</v>
+      </c>
+      <c r="J5" t="s">
+        <v>62</v>
+      </c>
+      <c r="K5" t="s">
+        <v>51</v>
+      </c>
+      <c r="L5" t="s">
+        <v>68</v>
+      </c>
+      <c r="M5" t="s">
+        <v>59</v>
+      </c>
+      <c r="N5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" t="s">
+        <v>48</v>
+      </c>
+      <c r="F6" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H6" t="s">
+        <v>58</v>
+      </c>
+      <c r="I6" t="s">
+        <v>59</v>
+      </c>
+      <c r="J6" t="s">
+        <v>60</v>
+      </c>
+      <c r="K6" t="s">
+        <v>65</v>
+      </c>
+      <c r="L6" t="s">
+        <v>69</v>
+      </c>
+      <c r="M6" t="s">
+        <v>59</v>
+      </c>
+      <c r="N6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" t="s">
         <v>49</v>
       </c>
-      <c r="L2" t="s">
+      <c r="F7" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" t="s">
+        <v>56</v>
+      </c>
+      <c r="H7" t="s">
+        <v>58</v>
+      </c>
+      <c r="I7" t="s">
+        <v>59</v>
+      </c>
+      <c r="J7" t="s">
+        <v>63</v>
+      </c>
+      <c r="K7" t="s">
+        <v>65</v>
+      </c>
+      <c r="L7" t="s">
+        <v>69</v>
+      </c>
+      <c r="M7" t="s">
+        <v>59</v>
+      </c>
+      <c r="N7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8" t="s">
+        <v>50</v>
+      </c>
+      <c r="F8" t="s">
+        <v>36</v>
+      </c>
+      <c r="G8" t="s">
+        <v>36</v>
+      </c>
+      <c r="H8" t="s">
+        <v>58</v>
+      </c>
+      <c r="I8" t="s">
+        <v>59</v>
+      </c>
+      <c r="J8" t="s">
+        <v>61</v>
+      </c>
+      <c r="K8" t="s">
+        <v>49</v>
+      </c>
+      <c r="L8" t="s">
         <v>67</v>
       </c>
-      <c r="M2" t="s">
-        <v>60</v>
-      </c>
-      <c r="N2" t="s">
-        <v>60</v>
-      </c>
-      <c r="O2">
-        <v>3</v>
+      <c r="M8" t="s">
+        <v>59</v>
+      </c>
+      <c r="N8" t="s">
+        <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
-      <c r="A3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D3" t="s">
-        <v>40</v>
-      </c>
-      <c r="E3" t="s">
+    <row r="9" spans="1:14">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9" t="s">
+        <v>51</v>
+      </c>
+      <c r="F9" t="s">
+        <v>37</v>
+      </c>
+      <c r="G9" t="s">
+        <v>57</v>
+      </c>
+      <c r="H9" t="s">
+        <v>58</v>
+      </c>
+      <c r="I9" t="s">
+        <v>59</v>
+      </c>
+      <c r="J9" t="s">
+        <v>64</v>
+      </c>
+      <c r="K9" t="s">
+        <v>65</v>
+      </c>
+      <c r="L9" t="s">
+        <v>69</v>
+      </c>
+      <c r="M9" t="s">
+        <v>59</v>
+      </c>
+      <c r="N9" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" t="s">
+        <v>46</v>
+      </c>
+      <c r="E10" t="s">
         <v>49</v>
       </c>
-      <c r="F3" t="s">
-        <v>32</v>
-      </c>
-      <c r="G3" t="s">
-        <v>54</v>
-      </c>
-      <c r="H3" t="s">
-        <v>59</v>
-      </c>
-      <c r="I3" t="s">
-        <v>60</v>
-      </c>
-      <c r="J3" t="s">
-        <v>61</v>
-      </c>
-      <c r="K3" t="s">
-        <v>51</v>
-      </c>
-      <c r="L3" t="s">
-        <v>67</v>
-      </c>
-      <c r="M3" t="s">
-        <v>60</v>
-      </c>
-      <c r="N3" t="s">
-        <v>60</v>
-      </c>
-      <c r="O3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15">
-      <c r="A4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D4" t="s">
-        <v>41</v>
-      </c>
-      <c r="E4" t="s">
-        <v>49</v>
-      </c>
-      <c r="F4" t="s">
-        <v>33</v>
-      </c>
-      <c r="G4" t="s">
-        <v>33</v>
-      </c>
-      <c r="H4" t="s">
-        <v>59</v>
-      </c>
-      <c r="I4" t="s">
-        <v>60</v>
-      </c>
-      <c r="J4" t="s">
-        <v>62</v>
-      </c>
-      <c r="K4" t="s">
-        <v>51</v>
-      </c>
-      <c r="L4" t="s">
-        <v>68</v>
-      </c>
-      <c r="M4" t="s">
-        <v>60</v>
-      </c>
-      <c r="N4" t="s">
-        <v>60</v>
-      </c>
-      <c r="O4">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15">
-      <c r="A5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D5" t="s">
-        <v>42</v>
-      </c>
-      <c r="E5" t="s">
-        <v>49</v>
-      </c>
-      <c r="F5" t="s">
-        <v>34</v>
-      </c>
-      <c r="G5" t="s">
-        <v>55</v>
-      </c>
-      <c r="H5" t="s">
-        <v>59</v>
-      </c>
-      <c r="I5" t="s">
-        <v>60</v>
-      </c>
-      <c r="J5" t="s">
+      <c r="F10" t="s">
+        <v>35</v>
+      </c>
+      <c r="G10" t="s">
+        <v>56</v>
+      </c>
+      <c r="H10" t="s">
+        <v>58</v>
+      </c>
+      <c r="I10" t="s">
+        <v>59</v>
+      </c>
+      <c r="J10" t="s">
         <v>63</v>
       </c>
-      <c r="K5" t="s">
-        <v>52</v>
-      </c>
-      <c r="L5" t="s">
+      <c r="K10" t="s">
+        <v>65</v>
+      </c>
+      <c r="L10" t="s">
         <v>69</v>
       </c>
-      <c r="M5" t="s">
-        <v>60</v>
-      </c>
-      <c r="N5" t="s">
-        <v>60</v>
-      </c>
-      <c r="O5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15">
-      <c r="A6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D6" t="s">
-        <v>43</v>
-      </c>
-      <c r="E6" t="s">
-        <v>49</v>
-      </c>
-      <c r="F6" t="s">
-        <v>35</v>
-      </c>
-      <c r="G6" t="s">
-        <v>56</v>
-      </c>
-      <c r="H6" t="s">
-        <v>59</v>
-      </c>
-      <c r="I6" t="s">
-        <v>60</v>
-      </c>
-      <c r="J6" t="s">
-        <v>61</v>
-      </c>
-      <c r="K6" t="s">
-        <v>66</v>
-      </c>
-      <c r="L6" t="s">
+      <c r="M10" t="s">
+        <v>59</v>
+      </c>
+      <c r="N10" t="s">
         <v>70</v>
-      </c>
-      <c r="M6" t="s">
-        <v>60</v>
-      </c>
-      <c r="N6" t="s">
-        <v>60</v>
-      </c>
-      <c r="O6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15">
-      <c r="A7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D7" t="s">
-        <v>44</v>
-      </c>
-      <c r="E7" t="s">
-        <v>50</v>
-      </c>
-      <c r="F7" t="s">
-        <v>36</v>
-      </c>
-      <c r="G7" t="s">
-        <v>57</v>
-      </c>
-      <c r="H7" t="s">
-        <v>59</v>
-      </c>
-      <c r="I7" t="s">
-        <v>60</v>
-      </c>
-      <c r="J7" t="s">
-        <v>64</v>
-      </c>
-      <c r="K7" t="s">
-        <v>66</v>
-      </c>
-      <c r="L7" t="s">
-        <v>70</v>
-      </c>
-      <c r="M7" t="s">
-        <v>60</v>
-      </c>
-      <c r="N7" t="s">
-        <v>71</v>
-      </c>
-      <c r="O7">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15">
-      <c r="A8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" t="s">
-        <v>37</v>
-      </c>
-      <c r="D8" t="s">
-        <v>45</v>
-      </c>
-      <c r="E8" t="s">
-        <v>51</v>
-      </c>
-      <c r="F8" t="s">
-        <v>37</v>
-      </c>
-      <c r="G8" t="s">
-        <v>37</v>
-      </c>
-      <c r="H8" t="s">
-        <v>59</v>
-      </c>
-      <c r="I8" t="s">
-        <v>60</v>
-      </c>
-      <c r="J8" t="s">
-        <v>62</v>
-      </c>
-      <c r="K8" t="s">
-        <v>50</v>
-      </c>
-      <c r="L8" t="s">
-        <v>68</v>
-      </c>
-      <c r="M8" t="s">
-        <v>60</v>
-      </c>
-      <c r="N8" t="s">
-        <v>60</v>
-      </c>
-      <c r="O8">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15">
-      <c r="A9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" t="s">
-        <v>30</v>
-      </c>
-      <c r="C9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D9" t="s">
-        <v>46</v>
-      </c>
-      <c r="E9" t="s">
-        <v>52</v>
-      </c>
-      <c r="F9" t="s">
-        <v>38</v>
-      </c>
-      <c r="G9" t="s">
-        <v>58</v>
-      </c>
-      <c r="H9" t="s">
-        <v>59</v>
-      </c>
-      <c r="I9" t="s">
-        <v>60</v>
-      </c>
-      <c r="J9" t="s">
-        <v>65</v>
-      </c>
-      <c r="K9" t="s">
-        <v>66</v>
-      </c>
-      <c r="L9" t="s">
-        <v>70</v>
-      </c>
-      <c r="M9" t="s">
-        <v>60</v>
-      </c>
-      <c r="N9" t="s">
-        <v>60</v>
-      </c>
-      <c r="O9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15">
-      <c r="A10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" t="s">
-        <v>36</v>
-      </c>
-      <c r="D10" t="s">
-        <v>47</v>
-      </c>
-      <c r="E10" t="s">
-        <v>50</v>
-      </c>
-      <c r="F10" t="s">
-        <v>36</v>
-      </c>
-      <c r="G10" t="s">
-        <v>57</v>
-      </c>
-      <c r="H10" t="s">
-        <v>59</v>
-      </c>
-      <c r="I10" t="s">
-        <v>60</v>
-      </c>
-      <c r="J10" t="s">
-        <v>64</v>
-      </c>
-      <c r="K10" t="s">
-        <v>66</v>
-      </c>
-      <c r="L10" t="s">
-        <v>70</v>
-      </c>
-      <c r="M10" t="s">
-        <v>60</v>
-      </c>
-      <c r="N10" t="s">
-        <v>71</v>
-      </c>
-      <c r="O10">
-        <v>-1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Parallel UD Match fixed for matching the pivot
The issue was on the join, which was performed based on the old index and not on the sorting that occurs right before..
</commit_message>
<xml_diff>
--- a/Xports/UD_French-FQB/VERB-indirect-obj.xlsx
+++ b/Xports/UD_French-FQB/VERB-indirect-obj.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="72">
   <si>
     <t>sent_id</t>
   </si>
@@ -58,6 +58,9 @@
     <t>MISC</t>
   </si>
   <si>
+    <t>dist</t>
+  </si>
+  <si>
     <t>FQB_CLEF03-118</t>
   </si>
   <si>
@@ -73,6 +76,9 @@
     <t>FQB_PoleEmploi-28</t>
   </si>
   <si>
+    <t>FQB_TREC-fr-1858-imp</t>
+  </si>
+  <si>
     <t>FQB_TREC-fr-403-imp</t>
   </si>
   <si>
@@ -82,9 +88,6 @@
     <t>FQB_TREC-fr-757</t>
   </si>
   <si>
-    <t>FQB_TREC-fr-1858-imp</t>
-  </si>
-  <si>
     <t xml:space="preserve">Quel est le nom de la station de métro où a </t>
   </si>
   <si>
@@ -145,6 +148,9 @@
     <t xml:space="preserve"> d'adhérer au CSP ? </t>
   </si>
   <si>
+    <t xml:space="preserve">-moi où est située la compagnie DuPont. </t>
+  </si>
+  <si>
     <t xml:space="preserve">-moi près de quelle ville se trouve le parc Kentucky Horse. </t>
   </si>
   <si>
@@ -152,9 +158,6 @@
   </si>
   <si>
     <t xml:space="preserve"> la plus grande quantité de caféine ? </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-moi où est située la compagnie DuPont. </t>
   </si>
   <si>
     <t>12</t>
@@ -584,13 +587,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N10"/>
+  <dimension ref="A1:O10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -633,280 +636,298 @@
       <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:15">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G2" t="s">
+        <v>53</v>
+      </c>
+      <c r="H2" t="s">
+        <v>59</v>
+      </c>
+      <c r="I2" t="s">
+        <v>60</v>
+      </c>
+      <c r="J2" t="s">
+        <v>61</v>
+      </c>
+      <c r="K2" t="s">
+        <v>49</v>
+      </c>
+      <c r="L2" t="s">
+        <v>67</v>
+      </c>
+      <c r="M2" t="s">
+        <v>60</v>
+      </c>
+      <c r="N2" t="s">
+        <v>60</v>
+      </c>
+      <c r="O2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" t="s">
+        <v>54</v>
+      </c>
+      <c r="H3" t="s">
+        <v>59</v>
+      </c>
+      <c r="I3" t="s">
+        <v>60</v>
+      </c>
+      <c r="J3" t="s">
+        <v>61</v>
+      </c>
+      <c r="K3" t="s">
+        <v>51</v>
+      </c>
+      <c r="L3" t="s">
+        <v>67</v>
+      </c>
+      <c r="M3" t="s">
+        <v>60</v>
+      </c>
+      <c r="N3" t="s">
+        <v>60</v>
+      </c>
+      <c r="O3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I4" t="s">
+        <v>60</v>
+      </c>
+      <c r="J4" t="s">
+        <v>62</v>
+      </c>
+      <c r="K4" t="s">
+        <v>51</v>
+      </c>
+      <c r="L4" t="s">
+        <v>68</v>
+      </c>
+      <c r="M4" t="s">
+        <v>60</v>
+      </c>
+      <c r="N4" t="s">
+        <v>60</v>
+      </c>
+      <c r="O4">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" t="s">
+        <v>55</v>
+      </c>
+      <c r="H5" t="s">
+        <v>59</v>
+      </c>
+      <c r="I5" t="s">
+        <v>60</v>
+      </c>
+      <c r="J5" t="s">
+        <v>63</v>
+      </c>
+      <c r="K5" t="s">
         <v>52</v>
       </c>
-      <c r="H2" t="s">
-        <v>58</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="L5" t="s">
+        <v>69</v>
+      </c>
+      <c r="M5" t="s">
+        <v>60</v>
+      </c>
+      <c r="N5" t="s">
+        <v>60</v>
+      </c>
+      <c r="O5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E6" t="s">
+        <v>49</v>
+      </c>
+      <c r="F6" t="s">
+        <v>35</v>
+      </c>
+      <c r="G6" t="s">
+        <v>56</v>
+      </c>
+      <c r="H6" t="s">
         <v>59</v>
       </c>
-      <c r="J2" t="s">
-        <v>60</v>
-      </c>
-      <c r="K2" t="s">
-        <v>48</v>
-      </c>
-      <c r="L2" t="s">
+      <c r="I6" t="s">
+        <v>60</v>
+      </c>
+      <c r="J6" t="s">
+        <v>61</v>
+      </c>
+      <c r="K6" t="s">
         <v>66</v>
       </c>
-      <c r="M2" t="s">
+      <c r="L6" t="s">
+        <v>70</v>
+      </c>
+      <c r="M6" t="s">
+        <v>60</v>
+      </c>
+      <c r="N6" t="s">
+        <v>60</v>
+      </c>
+      <c r="O6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F7" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" t="s">
+        <v>57</v>
+      </c>
+      <c r="H7" t="s">
         <v>59</v>
       </c>
-      <c r="N2" t="s">
-        <v>59</v>
+      <c r="I7" t="s">
+        <v>60</v>
+      </c>
+      <c r="J7" t="s">
+        <v>64</v>
+      </c>
+      <c r="K7" t="s">
+        <v>66</v>
+      </c>
+      <c r="L7" t="s">
+        <v>70</v>
+      </c>
+      <c r="M7" t="s">
+        <v>60</v>
+      </c>
+      <c r="N7" t="s">
+        <v>71</v>
+      </c>
+      <c r="O7">
+        <v>-1</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E3" t="s">
-        <v>48</v>
-      </c>
-      <c r="F3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G3" t="s">
-        <v>53</v>
-      </c>
-      <c r="H3" t="s">
-        <v>58</v>
-      </c>
-      <c r="I3" t="s">
-        <v>59</v>
-      </c>
-      <c r="J3" t="s">
-        <v>60</v>
-      </c>
-      <c r="K3" t="s">
-        <v>50</v>
-      </c>
-      <c r="L3" t="s">
-        <v>66</v>
-      </c>
-      <c r="M3" t="s">
-        <v>59</v>
-      </c>
-      <c r="N3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14">
-      <c r="A4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D4" t="s">
-        <v>40</v>
-      </c>
-      <c r="E4" t="s">
-        <v>48</v>
-      </c>
-      <c r="F4" t="s">
-        <v>32</v>
-      </c>
-      <c r="G4" t="s">
-        <v>32</v>
-      </c>
-      <c r="H4" t="s">
-        <v>58</v>
-      </c>
-      <c r="I4" t="s">
-        <v>59</v>
-      </c>
-      <c r="J4" t="s">
-        <v>61</v>
-      </c>
-      <c r="K4" t="s">
-        <v>50</v>
-      </c>
-      <c r="L4" t="s">
-        <v>67</v>
-      </c>
-      <c r="M4" t="s">
-        <v>59</v>
-      </c>
-      <c r="N4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14">
-      <c r="A5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D5" t="s">
-        <v>41</v>
-      </c>
-      <c r="E5" t="s">
-        <v>48</v>
-      </c>
-      <c r="F5" t="s">
-        <v>33</v>
-      </c>
-      <c r="G5" t="s">
-        <v>54</v>
-      </c>
-      <c r="H5" t="s">
-        <v>58</v>
-      </c>
-      <c r="I5" t="s">
-        <v>59</v>
-      </c>
-      <c r="J5" t="s">
-        <v>62</v>
-      </c>
-      <c r="K5" t="s">
-        <v>51</v>
-      </c>
-      <c r="L5" t="s">
-        <v>68</v>
-      </c>
-      <c r="M5" t="s">
-        <v>59</v>
-      </c>
-      <c r="N5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14">
-      <c r="A6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D6" t="s">
-        <v>42</v>
-      </c>
-      <c r="E6" t="s">
-        <v>48</v>
-      </c>
-      <c r="F6" t="s">
-        <v>34</v>
-      </c>
-      <c r="G6" t="s">
-        <v>55</v>
-      </c>
-      <c r="H6" t="s">
-        <v>58</v>
-      </c>
-      <c r="I6" t="s">
-        <v>59</v>
-      </c>
-      <c r="J6" t="s">
-        <v>60</v>
-      </c>
-      <c r="K6" t="s">
-        <v>65</v>
-      </c>
-      <c r="L6" t="s">
-        <v>69</v>
-      </c>
-      <c r="M6" t="s">
-        <v>59</v>
-      </c>
-      <c r="N6" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14">
-      <c r="A7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D7" t="s">
-        <v>43</v>
-      </c>
-      <c r="E7" t="s">
-        <v>49</v>
-      </c>
-      <c r="F7" t="s">
-        <v>35</v>
-      </c>
-      <c r="G7" t="s">
-        <v>56</v>
-      </c>
-      <c r="H7" t="s">
-        <v>58</v>
-      </c>
-      <c r="I7" t="s">
-        <v>59</v>
-      </c>
-      <c r="J7" t="s">
-        <v>63</v>
-      </c>
-      <c r="K7" t="s">
-        <v>65</v>
-      </c>
-      <c r="L7" t="s">
-        <v>69</v>
-      </c>
-      <c r="M7" t="s">
-        <v>59</v>
-      </c>
-      <c r="N7" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:15">
       <c r="A8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C8" t="s">
         <v>36</v>
       </c>
       <c r="D8" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E8" t="s">
         <v>50</v>
@@ -915,33 +936,36 @@
         <v>36</v>
       </c>
       <c r="G8" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="H8" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="I8" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="J8" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="K8" t="s">
-        <v>49</v>
+        <v>66</v>
       </c>
       <c r="L8" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="M8" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="N8" t="s">
-        <v>59</v>
+        <v>71</v>
+      </c>
+      <c r="O8">
+        <v>-1</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:15">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B9" t="s">
         <v>29</v>
@@ -950,7 +974,7 @@
         <v>37</v>
       </c>
       <c r="D9" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E9" t="s">
         <v>51</v>
@@ -959,69 +983,78 @@
         <v>37</v>
       </c>
       <c r="G9" t="s">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="H9" t="s">
+        <v>59</v>
+      </c>
+      <c r="I9" t="s">
+        <v>60</v>
+      </c>
+      <c r="J9" t="s">
+        <v>62</v>
+      </c>
+      <c r="K9" t="s">
+        <v>50</v>
+      </c>
+      <c r="L9" t="s">
+        <v>68</v>
+      </c>
+      <c r="M9" t="s">
+        <v>60</v>
+      </c>
+      <c r="N9" t="s">
+        <v>60</v>
+      </c>
+      <c r="O9">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" t="s">
+        <v>47</v>
+      </c>
+      <c r="E10" t="s">
+        <v>52</v>
+      </c>
+      <c r="F10" t="s">
+        <v>38</v>
+      </c>
+      <c r="G10" t="s">
         <v>58</v>
       </c>
-      <c r="I9" t="s">
+      <c r="H10" t="s">
         <v>59</v>
       </c>
-      <c r="J9" t="s">
-        <v>64</v>
-      </c>
-      <c r="K9" t="s">
+      <c r="I10" t="s">
+        <v>60</v>
+      </c>
+      <c r="J10" t="s">
         <v>65</v>
       </c>
-      <c r="L9" t="s">
-        <v>69</v>
-      </c>
-      <c r="M9" t="s">
-        <v>59</v>
-      </c>
-      <c r="N9" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14">
-      <c r="A10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" t="s">
-        <v>35</v>
-      </c>
-      <c r="D10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E10" t="s">
-        <v>49</v>
-      </c>
-      <c r="F10" t="s">
-        <v>35</v>
-      </c>
-      <c r="G10" t="s">
-        <v>56</v>
-      </c>
-      <c r="H10" t="s">
-        <v>58</v>
-      </c>
-      <c r="I10" t="s">
-        <v>59</v>
-      </c>
-      <c r="J10" t="s">
-        <v>63</v>
-      </c>
       <c r="K10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="L10" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="M10" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="N10" t="s">
-        <v>70</v>
+        <v>60</v>
+      </c>
+      <c r="O10">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>